<commit_message>
added may 31 data
</commit_message>
<xml_diff>
--- a/data-raw/auris_and_albicans/HYS7.xlsx
+++ b/data-raw/auris_and_albicans/HYS7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\Documents\B Lab\cross-tolerance\data-raw\auris_and_albicans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FECA6B2-DF0A-41B0-89FA-0A3F1DE4397F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A639AB2D-9DEA-4D44-9420-CFF0E3E9FCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{416B0376-EACE-4FE1-8614-EDCA28D0841F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="30">
   <si>
     <t>well</t>
   </si>
@@ -135,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +165,12 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -193,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -201,6 +207,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD7BE5E-5607-4174-8537-91D979FCA955}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,6 +901,342 @@
         <v>1</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>0.31150001290000001</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>5.3700000050000002E-2</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>0.18729999659999999</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>0.1500999928</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>0.1741999984</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>0.10109999779999999</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>0.15430000420000001</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>5.0999999050000001E-2</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>0.20520000159999999</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>0.15899999440000001</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>5.2200000730000001E-2</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>0.3131000102</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>5.2099999039999997E-2</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>0.4577000141</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>0.29910001159999999</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>0.1226999983</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>0.26940000060000002</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>0.1344999969</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>0.23849999899999999</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>5.0999999050000001E-2</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>0.30059999230000001</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>5.090000108E-2</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>0.31769999859999998</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>0.3258000016</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -901,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC13E9DF-09E4-407F-8366-BC4EEB418F27}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,6 +1602,342 @@
         <v>1</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>8.76000002E-2</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>5.2299998700000003E-2</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>0.1014999971</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>8.0099999899999996E-2</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>8.5900001229999995E-2</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>0.12129999700000001</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>9.7099997100000002E-2</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>5.7900000360000002E-2</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>9.3500003220000003E-2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>8.9599996809999999E-2</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>5.240000039E-2</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>0.11789999900000001</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>5.1500000060000002E-2</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>0.1096000001</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>9.009999782E-2</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>0.15119999649999999</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>0.1085999981</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>9.1799996790000005E-2</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>8.6900003249999996E-2</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>5.2900001410000001E-2</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>0.13959999379999999</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>5.3599998349999997E-2</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>0.1636999995</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>0.25679999590000002</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1266,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F8F75F-36F4-4DFB-86F0-ACB61B088856}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,6 +2303,342 @@
         <v>1</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>0.50360000130000004</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>5.4400000720000001E-2</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>0.23409999910000001</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>0.25290000439999999</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>0.34560000899999999</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>0.30540001389999999</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>0.26019999379999997</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>5.4400000720000001E-2</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>0.17790000140000001</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>0.1808000058</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>5.3300000729999998E-2</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>0.19740000369999999</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>5.1100000739999998E-2</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>0.23939999940000001</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>0.17880000169999999</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>0.1121999994</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>0.2036000043</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>0.1921000034</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>0.1682000011</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>5.2299998700000003E-2</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>0.16429999470000001</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>5.0700001420000002E-2</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>0.35289999840000003</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>0.36689999699999998</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1631,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3944297D-12CA-4BA2-B535-6673F8F0643F}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1989,6 +3004,342 @@
         <v>1</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>0.1948000044</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>5.2900001410000001E-2</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>0.4361999929</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>0.35640001300000002</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>0.1008000001</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>9.7000002860000004E-2</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>5.6699998680000002E-2</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>5.6499999019999997E-2</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>0.1238999963</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>0.1203999966</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>5.0599999729999998E-2</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>6.8800002339999999E-2</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>5.1699999720000001E-2</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>6.6299997269999994E-2</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>5.2000001070000003E-2</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>5.2799999709999997E-2</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>0.3454000056</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>0.25090000029999998</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>0.23299999539999999</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>5.2000001070000003E-2</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>0.32170000669999999</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>5.319999903E-2</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>0.29440000649999998</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>0.3819000125</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>